<commit_message>
Mise à jour avec le doodle + les interclubs.
</commit_message>
<xml_diff>
--- a/ListNageur.xlsx
+++ b/ListNageur.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="112">
   <si>
     <t>Jordan</t>
   </si>
@@ -22,13 +22,334 @@
     <t>Mosio</t>
   </si>
   <si>
-    <t>Valentin</t>
-  </si>
-  <si>
-    <t>Papereux</t>
-  </si>
-  <si>
-    <t>Solène</t>
+    <t>Florestan</t>
+  </si>
+  <si>
+    <t>Jaouen</t>
+  </si>
+  <si>
+    <t>Gerard</t>
+  </si>
+  <si>
+    <t>Philippe</t>
+  </si>
+  <si>
+    <t>Tournier</t>
+  </si>
+  <si>
+    <t>Marion</t>
+  </si>
+  <si>
+    <t>Sylvaine</t>
+  </si>
+  <si>
+    <t>Jenhani</t>
+  </si>
+  <si>
+    <t>Sylvie</t>
+  </si>
+  <si>
+    <t>Jacques</t>
+  </si>
+  <si>
+    <t>Michel</t>
+  </si>
+  <si>
+    <t>Pierre</t>
+  </si>
+  <si>
+    <t>Julie</t>
+  </si>
+  <si>
+    <t>Leuiller</t>
+  </si>
+  <si>
+    <t>Marianne</t>
+  </si>
+  <si>
+    <t>Baringou</t>
+  </si>
+  <si>
+    <t>Christelle</t>
+  </si>
+  <si>
+    <t>Ducruet</t>
+  </si>
+  <si>
+    <t>Pauline</t>
+  </si>
+  <si>
+    <t>Barthe</t>
+  </si>
+  <si>
+    <t>Olivier</t>
+  </si>
+  <si>
+    <t>Magnin</t>
+  </si>
+  <si>
+    <t>Cedric</t>
+  </si>
+  <si>
+    <t>Barret</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Hillers</t>
+  </si>
+  <si>
+    <t>Eliska</t>
+  </si>
+  <si>
+    <t>Zikmund</t>
+  </si>
+  <si>
+    <t>Gregor</t>
+  </si>
+  <si>
+    <t>Flavien</t>
+  </si>
+  <si>
+    <t>Hirigoyen</t>
+  </si>
+  <si>
+    <t>Adeline</t>
+  </si>
+  <si>
+    <t>Claire</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Murari</t>
+  </si>
+  <si>
+    <t>Julien</t>
+  </si>
+  <si>
+    <t>Sandrine</t>
+  </si>
+  <si>
+    <t>Serge</t>
+  </si>
+  <si>
+    <t>Damien</t>
+  </si>
+  <si>
+    <t>Goffin</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Isabelle</t>
+  </si>
+  <si>
+    <t>Païlan</t>
+  </si>
+  <si>
+    <t>Ilann</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Rebecchi</t>
+  </si>
+  <si>
+    <t>Besson</t>
+  </si>
+  <si>
+    <t>Bonvilain</t>
+  </si>
+  <si>
+    <t>Agnes</t>
+  </si>
+  <si>
+    <t>Bourgeois</t>
+  </si>
+  <si>
+    <t>Bevilacqua</t>
+  </si>
+  <si>
+    <t>Genevieve</t>
+  </si>
+  <si>
+    <t>Jerome</t>
+  </si>
+  <si>
+    <t>Beaucour</t>
+  </si>
+  <si>
+    <t>Borrel</t>
+  </si>
+  <si>
+    <t>Cartier</t>
+  </si>
+  <si>
+    <t>Chambon</t>
+  </si>
+  <si>
+    <t>Croset</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Aurelien</t>
+  </si>
+  <si>
+    <t>Despax</t>
+  </si>
+  <si>
+    <t>Fellini</t>
+  </si>
+  <si>
+    <t>Hennion</t>
+  </si>
+  <si>
+    <t>Antoine</t>
+  </si>
+  <si>
+    <t>Karim</t>
+  </si>
+  <si>
+    <t>Cecile</t>
+  </si>
+  <si>
+    <t>Melanie</t>
+  </si>
+  <si>
+    <t>Legrais</t>
+  </si>
+  <si>
+    <t>Leval</t>
+  </si>
+  <si>
+    <t>Christele</t>
+  </si>
+  <si>
+    <t>Zaslavoglou</t>
+  </si>
+  <si>
+    <t>Anne-sophie</t>
+  </si>
+  <si>
+    <t>Seroi</t>
+  </si>
+  <si>
+    <t>Sprich</t>
+  </si>
+  <si>
+    <t>Elisabeth</t>
+  </si>
+  <si>
+    <t>Boris</t>
+  </si>
+  <si>
+    <t>Cédric</t>
+  </si>
+  <si>
+    <t>Mortini</t>
+  </si>
+  <si>
+    <t>Bénédicte</t>
+  </si>
+  <si>
+    <t>Desmaris</t>
+  </si>
+  <si>
+    <t>Deroin</t>
+  </si>
+  <si>
+    <t>Chidlovskii</t>
+  </si>
+  <si>
+    <t>Crochet</t>
+  </si>
+  <si>
+    <t>Desmons</t>
+  </si>
+  <si>
+    <t>Lesbordes</t>
+  </si>
+  <si>
+    <t>Miscioscia</t>
+  </si>
+  <si>
+    <t>Demenditte</t>
+  </si>
+  <si>
+    <t>Clement</t>
+  </si>
+  <si>
+    <t>Caroline</t>
+  </si>
+  <si>
+    <t>De Lamberterie</t>
+  </si>
+  <si>
+    <t>Yoann</t>
+  </si>
+  <si>
+    <t>Joury</t>
+  </si>
+  <si>
+    <t>Le Comte</t>
+  </si>
+  <si>
+    <t>Lapouge</t>
+  </si>
+  <si>
+    <t>Le Fol</t>
+  </si>
+  <si>
+    <t>Noel Rist</t>
+  </si>
+  <si>
+    <t>Poggi</t>
+  </si>
+  <si>
+    <t>Planat</t>
+  </si>
+  <si>
+    <t>Redjadj</t>
+  </si>
+  <si>
+    <t>Rigal</t>
+  </si>
+  <si>
+    <t>Spilliaert</t>
+  </si>
+  <si>
+    <t>Vivo</t>
+  </si>
+  <si>
+    <t>Vigneron</t>
+  </si>
+  <si>
+    <t>Yann</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Duhet Mattera</t>
+  </si>
+  <si>
+    <t>Frédéric</t>
+  </si>
+  <si>
+    <t>Nathalia</t>
+  </si>
+  <si>
+    <t>Deroin-Hervet</t>
+  </si>
+  <si>
+    <t>Soazic</t>
   </si>
 </sst>
 </file>
@@ -64,8 +385,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,39 +694,507 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B44" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="A1:B61">
+    <sortCondition ref="B1:B61"/>
+    <sortCondition ref="A1:A61"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Affichage plus joli de la solution.
</commit_message>
<xml_diff>
--- a/ListNageur.xlsx
+++ b/ListNageur.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
   <si>
     <t>Jordan</t>
   </si>
@@ -350,6 +350,21 @@
   </si>
   <si>
     <t>Soazic</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Tonnerre</t>
+  </si>
+  <si>
+    <t>Villet</t>
+  </si>
+  <si>
+    <t>Laurent</t>
+  </si>
+  <si>
+    <t>Dillmann</t>
   </si>
 </sst>
 </file>
@@ -694,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,55 +899,55 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>107</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>27</v>
@@ -940,31 +955,31 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>93</v>
@@ -972,159 +987,159 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>74</v>
@@ -1132,62 +1147,86 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:B61">

</xml_diff>